<commit_message>
updated file according to finished tasks
</commit_message>
<xml_diff>
--- a/for_developers/Liste_FE_Functions_Testcoverage.xlsx
+++ b/for_developers/Liste_FE_Functions_Testcoverage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\Desktop\TEMP-FP7.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
   <si>
     <t>ControlFile</t>
   </si>
@@ -34,9 +33,6 @@
     <t>__init__</t>
   </si>
   <si>
-    <t>__read_controlfile__</t>
-  </si>
-  <si>
     <t>__str__</t>
   </si>
   <si>
@@ -64,9 +60,6 @@
     <t>Class or Module</t>
   </si>
   <si>
-    <t>move to install module</t>
-  </si>
-  <si>
     <t>EcFlexpart</t>
   </si>
   <si>
@@ -76,9 +69,6 @@
     <t>_start_retrievement</t>
   </si>
   <si>
-    <t>rename with just one leading _</t>
-  </si>
-  <si>
     <t>_mk_index_values</t>
   </si>
   <si>
@@ -103,9 +93,6 @@
     <t>GribTools</t>
   </si>
   <si>
-    <t>rename Classname</t>
-  </si>
-  <si>
     <t>get_keys</t>
   </si>
   <si>
@@ -133,9 +120,6 @@
     <t>data_retrieve</t>
   </si>
   <si>
-    <t>do we stil need it?</t>
-  </si>
-  <si>
     <t>UioFiles</t>
   </si>
   <si>
@@ -166,9 +150,6 @@
     <t>do_retrievement</t>
   </si>
   <si>
-    <t>rename function</t>
-  </si>
-  <si>
     <t>prepare_flexpart</t>
   </si>
   <si>
@@ -202,15 +183,6 @@
     <t>make_convert_build</t>
   </si>
   <si>
-    <t>rename from to del</t>
-  </si>
-  <si>
-    <t>rename to mk</t>
-  </si>
-  <si>
-    <t>rename to args</t>
-  </si>
-  <si>
     <t>profiling</t>
   </si>
   <si>
@@ -268,9 +240,6 @@
     <t>submit_job_to_ecserver</t>
   </si>
   <si>
-    <t xml:space="preserve">rename to rm </t>
-  </si>
-  <si>
     <t>classes</t>
   </si>
   <si>
@@ -305,6 +274,9 @@
   </si>
   <si>
     <t>Has to have the same amount of values as in TYPE!</t>
+  </si>
+  <si>
+    <t>_read_controlfile</t>
   </si>
 </sst>
 </file>
@@ -628,7 +600,7 @@
   <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,25 +614,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -673,48 +645,42 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -722,89 +688,86 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
@@ -812,30 +775,27 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -843,376 +803,352 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>45</v>
-      </c>
-      <c r="C46" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>49</v>
-      </c>
-      <c r="C52" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D54" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E54" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D55" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E55" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D56" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E56" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D57" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E57" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D58" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E58" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>56</v>
-      </c>
-      <c r="C59" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>57</v>
-      </c>
-      <c r="C60" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B64" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D67" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E67" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D68" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E68" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>67</v>
-      </c>
-      <c r="C69" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D69" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E69" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D70" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E70" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D71" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E71" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D72" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E72" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D73" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E73" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D74" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E74" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D75" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E75" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D76" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E76" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D77" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E77" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D78" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E78" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D79" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E79" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>77</v>
-      </c>
-      <c r="C80" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D80" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E80" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D81" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E81" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D82" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E82" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1239,7 +1175,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1247,71 +1183,71 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>